<commit_message>
updated the workplan file
</commit_message>
<xml_diff>
--- a/workplan.xlsx
+++ b/workplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rjob\Yes_SA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{417C154B-B8D0-4711-9471-79C13E1B31A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F706BFA3-9671-46F0-AB80-3328B0496F13}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10233" xr2:uid="{E5F56421-CC85-4583-A073-BB1099073FEB}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>Youth</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Country</t>
   </si>
@@ -36,9 +33,6 @@
     <t>Dollar sign change</t>
   </si>
   <si>
-    <t>youth</t>
-  </si>
-  <si>
     <t>age limit</t>
   </si>
   <si>
@@ -54,18 +48,59 @@
     <t>What to do</t>
   </si>
   <si>
-    <t>pyschomettrics</t>
-  </si>
-  <si>
     <t>remove the pop up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pyschometrics </t>
+  </si>
+  <si>
+    <t>add weekly and monthly windows</t>
+  </si>
+  <si>
+    <t>add placed summary on top left</t>
+  </si>
+  <si>
+    <t>add top performing companies</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {how do we say a company is top / what do we consider}</t>
+  </si>
+  <si>
+    <t>Engagements</t>
+  </si>
+  <si>
+    <t>Youth Demographics</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>add top performing youth {high answered/expected}</t>
+  </si>
+  <si>
+    <t>do we have a minimum placed time</t>
+  </si>
+  <si>
+    <t>Weekly and Monthly histograms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,7 +122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -95,13 +130,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,67 +462,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC75E285-5147-4A2D-86FC-4536BF94AD63}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="15.9375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.64453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.17578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.52734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.76171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some graph instructions and a list of modules as they appear on gnowbe
</commit_message>
<xml_diff>
--- a/workplan.xlsx
+++ b/workplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rjob\Yes_SA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Karis/Desktop/Git/YES_SA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F706BFA3-9671-46F0-AB80-3328B0496F13}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5275D2-127F-734F-A52D-4002C4085662}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10233" xr2:uid="{E5F56421-CC85-4583-A073-BB1099073FEB}"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="25600" windowHeight="10240" xr2:uid="{E5F56421-CC85-4583-A073-BB1099073FEB}"/>
   </bookViews>
   <sheets>
     <sheet name="workplan_dashboard" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Country</t>
   </si>
@@ -85,6 +85,60 @@
   </si>
   <si>
     <t>Weekly and Monthly histograms</t>
+  </si>
+  <si>
+    <t>Internal view Widget</t>
+  </si>
+  <si>
+    <t>Phone delivery</t>
+  </si>
+  <si>
+    <t>By placed youths, show phone delivery (What proportion of youths have phones)</t>
+  </si>
+  <si>
+    <t>Could use a pie chart.</t>
+  </si>
+  <si>
+    <t>Weekly survey</t>
+  </si>
+  <si>
+    <t>By youths with phones, show weekly survey engagement (Those with phones and have atleast done a survey)</t>
+  </si>
+  <si>
+    <t>Monthly survey</t>
+  </si>
+  <si>
+    <t>By youths with phones, show monthly survey engagement (Those with at least a monthly survey)</t>
+  </si>
+  <si>
+    <t>Survey counter</t>
+  </si>
+  <si>
+    <t>Have the survey counters on top</t>
+  </si>
+  <si>
+    <t>Not sure if we need this as its on the app engagement dashboard.</t>
+  </si>
+  <si>
+    <t>Gnowbe engagement</t>
+  </si>
+  <si>
+    <t>Show the proportion of youths with phones that have a module done</t>
+  </si>
+  <si>
+    <t>Will need to merge the gnowbe data with placed youths data first. This url from the ones Xen sent will give the gnowbe data (https://data.yes4youth.co.za/GlobalOverallLearning?csv=1)</t>
+  </si>
+  <si>
+    <t>Gnowbe module counter</t>
+  </si>
+  <si>
+    <t>We need to show per module counter</t>
+  </si>
+  <si>
+    <t>We can have a bar graph showing the proportion of placed youths with phones who have done each module. We have 9 modules on the app so we can show the percentages by each module. Will send you a list of the modules.</t>
+  </si>
+  <si>
+    <t>Remember generating the files for the inconsistencies you find.</t>
   </si>
 </sst>
 </file>
@@ -143,11 +197,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,20 +519,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC75E285-5147-4A2D-86FC-4536BF94AD63}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.17578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.52734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.76171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="142.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -486,7 +543,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -494,7 +551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -502,7 +559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -513,7 +570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -521,7 +578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -529,7 +586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -537,7 +594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -545,7 +602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -556,7 +613,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -567,7 +624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -575,7 +632,81 @@
         <v>19</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A14:B14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated the pyschometrics histograms
</commit_message>
<xml_diff>
--- a/workplan.xlsx
+++ b/workplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Karis/Desktop/Git/YES_SA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rjob\Yes_SA\YES_shiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5275D2-127F-734F-A52D-4002C4085662}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4ECC92BE-B9F0-40DD-8A5A-2E2BC19B49CF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="460" windowWidth="25600" windowHeight="10240" xr2:uid="{E5F56421-CC85-4583-A073-BB1099073FEB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Country</t>
   </si>
@@ -139,13 +139,22 @@
   </si>
   <si>
     <t>Remember generating the files for the inconsistencies you find.</t>
+  </si>
+  <si>
+    <t>Download button</t>
+  </si>
+  <si>
+    <t>percentages of youths completing each module and dissaggregate by company</t>
+  </si>
+  <si>
+    <t>(https://data.yes4youth.co.za/GlobalOverallLearning?csv=1) {george email}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +166,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -194,10 +211,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -205,8 +223,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -519,20 +539,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC75E285-5147-4A2D-86FC-4536BF94AD63}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="142.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.17578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.46875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="142.64453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -543,7 +563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -551,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -559,7 +579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -570,7 +590,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -578,7 +598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -586,7 +606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -594,7 +614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -602,7 +622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -613,7 +633,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -624,7 +644,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -632,82 +652,104 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B23" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B27" t="s">
         <v>32</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
         <v>34</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B28" t="s">
         <v>35</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A22:B22"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C13" r:id="rId1" display="https://data.yes4youth.co.za/GlobalOverallLearning?csv=1" xr:uid="{18EEBA51-4EA4-4808-BEF5-D9EC112289A6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>